<commit_message>
export base-package aliases previously missed, dialogs.R functions previously missed, stats.R functions previously missed, update excel spreadsheet with constants, and add graphics-package aliases file.
</commit_message>
<xml_diff>
--- a/other/constants.xlsx
+++ b/other/constants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmartineau/j-martineau/uj/other/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D16AD87-0921-AC43-AA3C-DAD4A9305C7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27346A4F-1534-5E4D-8B12-9A08DFDE7E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="27460" windowHeight="16940" xr2:uid="{9423F248-3048-204A-B09D-EB0E672E0F08}"/>
   </bookViews>
@@ -74,25 +74,25 @@
     <t>c(letters, LETTERS)</t>
   </si>
   <si>
-    <t>c(letters, LETTERS, 0:9, '.')</t>
-  </si>
-  <si>
-    <t>c(letters, LETTERS, 0:9, '_', '.', ' ', ',', '-', '(', ')')</t>
-  </si>
-  <si>
-    <t>c(letters, LETTERS, 0:9, '.', ' ', ',', '-', '(', ')')</t>
-  </si>
-  <si>
-    <t>c(letters, LETTERS, 0:9, '.', ' ', '×', '+', '*', ':')</t>
-  </si>
-  <si>
-    <t>c('a', 'e', 'i', 'o', 'u', 'A', 'E', 'I', 'O', 'U')</t>
+    <t>c(letters, LETTERS, 0:9, "_", ".")</t>
+  </si>
+  <si>
+    <t>c(letters, LETTERS, 0:9, ".")</t>
+  </si>
+  <si>
+    <t>c(letters, LETTERS, 0:9, "_", ".", " ", ",", "-", "(", ")")</t>
+  </si>
+  <si>
+    <t>c(letters, LETTERS, 0:9, ".", " ", ",", "-", "(", ")")</t>
+  </si>
+  <si>
+    <t>c(letters, LETTERS, 0:9, ".", " ", "×", "+", "*", ":")</t>
+  </si>
+  <si>
+    <t>c("a", "e", "i", "o", "u", "A", "E", "I", "O", "U")</t>
   </si>
   <si>
     <t>c('solid', '42', '22', '11', '4111', '2111', '1114', '1112', '1441')</t>
-  </si>
-  <si>
-    <t>c(letters, LETTERS, 0:9, '_', '.')</t>
   </si>
   <si>
     <t>name</t>
@@ -3303,7 +3303,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3313,11 +3313,16 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="10"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Monaco"/>
       <family val="2"/>
-      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Monaco"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -3340,14 +3345,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3664,310 +3670,282 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9B7F589-33AD-F946-B4D0-A23240EB81A3}">
   <dimension ref="A1:NX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="NT1" workbookViewId="0">
-      <selection activeCell="NY1" sqref="NY1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:NX2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="35.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.33203125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="40.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="13" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="15" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="15" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="16" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="29.1640625" bestFit="1" customWidth="1"/>
-    <col min="61" max="61" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="27.6640625" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="36.1640625" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="23.6640625" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="77" max="78" width="8" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="82" max="82" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="84" max="92" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="93" max="94" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="95" max="95" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="97" max="97" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="98" max="98" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="99" max="107" width="9" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="109" max="109" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="110" max="110" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="112" max="112" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="113" max="114" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="115" max="115" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="116" max="116" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="118" max="118" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="119" max="119" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="121" max="121" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="122" max="122" width="14" bestFit="1" customWidth="1"/>
-    <col min="123" max="124" width="11" bestFit="1" customWidth="1"/>
-    <col min="125" max="125" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="11" bestFit="1" customWidth="1"/>
-    <col min="127" max="127" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="128" max="130" width="11" bestFit="1" customWidth="1"/>
-    <col min="131" max="131" width="13" bestFit="1" customWidth="1"/>
-    <col min="132" max="140" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="141" max="142" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="143" max="143" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="144" max="144" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="145" max="145" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="146" max="146" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="147" max="155" width="13" bestFit="1" customWidth="1"/>
-    <col min="156" max="157" width="9" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="9" bestFit="1" customWidth="1"/>
-    <col min="160" max="160" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="161" max="164" width="9" bestFit="1" customWidth="1"/>
-    <col min="165" max="165" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="166" max="166" width="10" bestFit="1" customWidth="1"/>
-    <col min="167" max="167" width="9" bestFit="1" customWidth="1"/>
-    <col min="168" max="168" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="169" max="169" width="9" bestFit="1" customWidth="1"/>
-    <col min="170" max="170" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="171" max="174" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="175" max="175" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="176" max="178" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="179" max="179" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="180" max="180" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="181" max="181" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="182" max="182" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="183" max="183" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="184" max="184" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="185" max="185" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="186" max="186" width="11" bestFit="1" customWidth="1"/>
-    <col min="187" max="187" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="188" max="188" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="189" max="189" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="190" max="190" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="191" max="191" width="11" bestFit="1" customWidth="1"/>
-    <col min="192" max="192" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="193" max="193" width="11" bestFit="1" customWidth="1"/>
-    <col min="194" max="194" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="195" max="196" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="197" max="197" width="13" bestFit="1" customWidth="1"/>
-    <col min="198" max="198" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="200" max="202" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="203" max="203" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="204" max="205" width="13" bestFit="1" customWidth="1"/>
-    <col min="206" max="206" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="207" max="207" width="13" bestFit="1" customWidth="1"/>
-    <col min="208" max="208" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="209" max="212" width="13" bestFit="1" customWidth="1"/>
-    <col min="213" max="213" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="214" max="214" width="14" bestFit="1" customWidth="1"/>
-    <col min="215" max="215" width="13" bestFit="1" customWidth="1"/>
-    <col min="216" max="216" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="217" max="217" width="13" bestFit="1" customWidth="1"/>
-    <col min="218" max="218" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="219" max="222" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="223" max="223" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="224" max="226" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="230" max="230" width="24.1640625" bestFit="1" customWidth="1"/>
-    <col min="231" max="231" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="232" max="232" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="233" max="233" width="26" bestFit="1" customWidth="1"/>
-    <col min="234" max="234" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="235" max="235" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="236" max="236" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="237" max="237" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="238" max="238" width="23" bestFit="1" customWidth="1"/>
-    <col min="239" max="239" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="240" max="250" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="251" max="251" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="252" max="252" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="253" max="253" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="254" max="254" width="13" bestFit="1" customWidth="1"/>
-    <col min="255" max="255" width="14" bestFit="1" customWidth="1"/>
-    <col min="256" max="256" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="257" max="257" width="15" bestFit="1" customWidth="1"/>
-    <col min="258" max="258" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="259" max="259" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="260" max="260" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="261" max="261" width="14" bestFit="1" customWidth="1"/>
-    <col min="262" max="262" width="15" bestFit="1" customWidth="1"/>
-    <col min="263" max="263" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="264" max="264" width="16" bestFit="1" customWidth="1"/>
-    <col min="265" max="265" width="13" bestFit="1" customWidth="1"/>
-    <col min="266" max="266" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="267" max="267" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="268" max="268" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="269" max="269" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="270" max="270" width="21" bestFit="1" customWidth="1"/>
-    <col min="271" max="271" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="272" max="272" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="273" max="273" width="19" bestFit="1" customWidth="1"/>
-    <col min="274" max="274" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="275" max="275" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="276" max="276" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="277" max="277" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="278" max="278" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="279" max="279" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="280" max="280" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="281" max="281" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="282" max="292" width="32" bestFit="1" customWidth="1"/>
-    <col min="293" max="293" width="29" bestFit="1" customWidth="1"/>
-    <col min="294" max="294" width="44.83203125" bestFit="1" customWidth="1"/>
-    <col min="295" max="295" width="31" bestFit="1" customWidth="1"/>
-    <col min="296" max="296" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="297" max="297" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="298" max="298" width="35" bestFit="1" customWidth="1"/>
-    <col min="299" max="299" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="300" max="300" width="30.1640625" bestFit="1" customWidth="1"/>
-    <col min="301" max="301" width="33" bestFit="1" customWidth="1"/>
-    <col min="302" max="302" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="303" max="303" width="32.33203125" bestFit="1" customWidth="1"/>
-    <col min="304" max="304" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="305" max="305" width="36" bestFit="1" customWidth="1"/>
-    <col min="306" max="306" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="307" max="307" width="31.1640625" bestFit="1" customWidth="1"/>
-    <col min="308" max="308" width="34" bestFit="1" customWidth="1"/>
-    <col min="309" max="309" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="310" max="310" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="311" max="311" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="312" max="312" width="39.33203125" bestFit="1" customWidth="1"/>
-    <col min="313" max="313" width="37.6640625" bestFit="1" customWidth="1"/>
-    <col min="314" max="314" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="315" max="315" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="316" max="316" width="32" bestFit="1" customWidth="1"/>
-    <col min="317" max="317" width="32.1640625" bestFit="1" customWidth="1"/>
-    <col min="318" max="318" width="33.1640625" bestFit="1" customWidth="1"/>
-    <col min="319" max="319" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="320" max="320" width="34.1640625" bestFit="1" customWidth="1"/>
-    <col min="321" max="321" width="31" bestFit="1" customWidth="1"/>
-    <col min="322" max="322" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="323" max="323" width="29" bestFit="1" customWidth="1"/>
-    <col min="324" max="334" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="335" max="335" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="336" max="336" width="45.33203125" bestFit="1" customWidth="1"/>
-    <col min="337" max="337" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="338" max="338" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="339" max="339" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="340" max="340" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="341" max="341" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="342" max="342" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="343" max="343" width="33.5" bestFit="1" customWidth="1"/>
-    <col min="344" max="344" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="345" max="345" width="32.83203125" bestFit="1" customWidth="1"/>
-    <col min="346" max="346" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="347" max="347" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="348" max="348" width="34.83203125" bestFit="1" customWidth="1"/>
-    <col min="349" max="349" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="350" max="350" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="351" max="351" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="352" max="352" width="36" bestFit="1" customWidth="1"/>
-    <col min="353" max="353" width="37.1640625" bestFit="1" customWidth="1"/>
-    <col min="354" max="354" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="355" max="355" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="356" max="356" width="35" bestFit="1" customWidth="1"/>
-    <col min="357" max="357" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="358" max="358" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="359" max="359" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="360" max="360" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="361" max="361" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="362" max="362" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="363" max="363" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="364" max="364" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="365" max="365" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="366" max="366" width="11.1640625" bestFit="1" customWidth="1"/>
-    <col min="367" max="367" width="15" bestFit="1" customWidth="1"/>
-    <col min="368" max="368" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="369" max="369" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="370" max="370" width="12" bestFit="1" customWidth="1"/>
-    <col min="371" max="371" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="372" max="373" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="374" max="374" width="116.1640625" bestFit="1" customWidth="1"/>
-    <col min="375" max="375" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="376" max="376" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="377" max="377" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="378" max="378" width="40.6640625" bestFit="1" customWidth="1"/>
-    <col min="379" max="379" width="30.5" bestFit="1" customWidth="1"/>
-    <col min="380" max="380" width="18" bestFit="1" customWidth="1"/>
-    <col min="381" max="381" width="16.83203125" bestFit="1" customWidth="1"/>
-    <col min="382" max="382" width="48" bestFit="1" customWidth="1"/>
-    <col min="383" max="383" width="48.33203125" bestFit="1" customWidth="1"/>
-    <col min="384" max="384" width="39.5" bestFit="1" customWidth="1"/>
-    <col min="385" max="385" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="386" max="386" width="35.83203125" bestFit="1" customWidth="1"/>
-    <col min="387" max="387" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="388" max="388" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="43.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="44.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="46.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="43.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="28.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="30.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="22.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="51" max="52" width="24.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="57" max="57" width="32.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="33.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="32.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="33.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="22.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="23.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="31.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="33.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="42.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="28.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="29.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="25.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="77" max="78" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="11.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="30.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="82" max="82" width="8.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="84" max="87" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="89" max="97" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="98" max="98" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="99" max="102" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="103" max="103" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="104" max="107" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="109" max="109" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="110" max="111" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="112" max="112" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="113" max="113" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="115" max="115" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="116" max="116" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="118" max="118" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="119" max="121" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="122" max="122" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="124" max="124" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="125" max="125" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="127" max="127" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="128" max="130" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="132" max="135" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="136" max="136" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="137" max="141" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="143" max="145" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="146" max="146" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="147" max="150" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="151" max="151" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="152" max="155" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="156" max="159" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="160" max="160" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="161" max="169" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="170" max="170" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="171" max="174" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="175" max="175" width="10.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="176" max="179" width="9.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="180" max="180" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="182" max="183" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="184" max="184" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="185" max="185" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="186" max="186" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="187" max="187" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="188" max="188" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="189" max="189" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="190" max="190" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="191" max="193" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="194" max="194" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="195" max="195" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="196" max="196" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="197" max="197" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="198" max="198" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="199" max="199" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="200" max="202" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="203" max="203" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="204" max="207" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="208" max="208" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="209" max="213" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="214" max="214" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="215" max="217" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="218" max="218" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="219" max="222" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="223" max="223" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="224" max="227" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="23.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="22.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="230" max="230" width="26.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="231" max="231" width="27.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="232" max="232" width="28.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="233" max="233" width="29.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="234" max="234" width="31.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="235" max="235" width="22.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="236" max="236" width="32.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="237" max="237" width="23.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="238" max="238" width="25.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="239" max="239" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="240" max="250" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="251" max="251" width="12.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="252" max="252" width="32.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="253" max="254" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="255" max="255" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="256" max="256" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="257" max="257" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="258" max="258" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="259" max="259" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="260" max="261" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="262" max="262" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="263" max="263" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="264" max="264" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="265" max="265" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="266" max="266" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="267" max="268" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="269" max="269" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="270" max="270" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="271" max="271" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="272" max="272" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="273" max="273" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="274" max="275" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="276" max="276" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="277" max="277" width="19.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="278" max="278" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="279" max="279" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="280" max="280" width="18.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="281" max="281" width="31.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="282" max="292" width="34.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="293" max="293" width="31.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="294" max="294" width="52.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="295" max="296" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="297" max="297" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="298" max="298" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="299" max="299" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="300" max="300" width="34.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="301" max="301" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="302" max="303" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="304" max="304" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="305" max="305" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="306" max="306" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="307" max="307" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="308" max="308" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="309" max="310" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="311" max="311" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="312" max="312" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="313" max="313" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="314" max="314" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="315" max="315" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="316" max="317" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="318" max="318" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="319" max="319" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="320" max="320" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="321" max="321" width="34.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="322" max="322" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="323" max="323" width="33.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="324" max="334" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="335" max="335" width="33.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="336" max="336" width="53.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="337" max="338" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="339" max="339" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="340" max="340" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="341" max="341" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="342" max="342" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="343" max="343" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="344" max="345" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="346" max="346" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="347" max="347" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="348" max="348" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="349" max="349" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="350" max="350" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="351" max="352" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="353" max="353" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="354" max="354" width="42.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="355" max="355" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="356" max="356" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="357" max="357" width="41" style="3" bestFit="1" customWidth="1"/>
+    <col min="358" max="359" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="360" max="360" width="38" style="3" bestFit="1" customWidth="1"/>
+    <col min="361" max="361" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="362" max="362" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="363" max="363" width="35.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="364" max="364" width="39" style="3" bestFit="1" customWidth="1"/>
+    <col min="365" max="365" width="48.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="366" max="366" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="367" max="367" width="17.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="368" max="368" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="369" max="369" width="15.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="370" max="370" width="13.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="371" max="371" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="372" max="373" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="374" max="374" width="141.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="375" max="375" width="71" style="3" bestFit="1" customWidth="1"/>
+    <col min="376" max="376" width="42.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="377" max="377" width="40" style="3" bestFit="1" customWidth="1"/>
+    <col min="378" max="378" width="48.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="379" max="379" width="37" style="3" bestFit="1" customWidth="1"/>
+    <col min="380" max="380" width="22.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="381" max="381" width="20.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="382" max="383" width="55.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="384" max="384" width="61.6640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="385" max="387" width="56.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="388" max="388" width="53.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="389" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:388" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:388" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -5133,7 +5111,7 @@
         <v>1080</v>
       </c>
     </row>
-    <row r="2" spans="1:388" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:388" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
@@ -6257,7 +6235,7 @@
         <v>32</v>
       </c>
       <c r="NK2" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="NL2" s="2" t="s">
         <v>6</v>
@@ -6278,28 +6256,28 @@
         <v>11</v>
       </c>
       <c r="NR2" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="NS2" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="NT2" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="NU2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="NV2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="NW2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="NW2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="NX2" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:388" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:388" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>21</v>
       </c>

</xml_diff>